<commit_message>
Updated plan for Controller.
</commit_message>
<xml_diff>
--- a/high_level_plan.xlsx
+++ b/high_level_plan.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="49">
   <si>
     <t xml:space="preserve">Capstone project by ‘The Distracted’</t>
   </si>
@@ -229,7 +229,22 @@
     <t xml:space="preserve">PID controller</t>
   </si>
   <si>
+    <t xml:space="preserve">Control – DBW Node</t>
+  </si>
+  <si>
     <t xml:space="preserve">The PID constants using Twiddle/etc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Twist controller</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is the main thing which needs to be coded</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DBW Node</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invoke Twist Controller and call publish</t>
   </si>
 </sst>
 </file>
@@ -364,10 +379,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C27" activeCellId="1" sqref="C26 C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -603,10 +618,32 @@
         <v>42</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="C25" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B26" s="0" t="s">
         <v>43</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>